<commit_message>
STO-260 #comment upload xls functionality in price grid #time 5h 30m upload xls functionality in price grid
</commit_message>
<xml_diff>
--- a/api/addpricegrid.xlsx
+++ b/api/addpricegrid.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="208" firstSheet="0" activeTab="6"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="208" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="PriceGrid" sheetId="1" state="visible" r:id="rId2"/>
@@ -17,18 +17,19 @@
     <sheet name="Embroidery Price" sheetId="7" state="visible" r:id="rId8"/>
     <sheet name="Direct To Garment" sheetId="8" state="visible" r:id="rId9"/>
     <sheet name="Garment Markup" sheetId="9" state="visible" r:id="rId10"/>
+    <sheet name="Sheet10" sheetId="10" state="visible" r:id="rId11"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="72">
   <si>
     <t>Name</t>
   </si>
   <si>
-    <t>Test Price Grid</t>
+    <t>Test Uploaded price grid</t>
   </si>
   <si>
     <t>Discharge</t>
@@ -106,31 +107,40 @@
     <t>Embroidery Names</t>
   </si>
   <si>
+    <t>Over Size Screens</t>
+  </si>
+  <si>
+    <t>Tag Removal</t>
+  </si>
+  <si>
+    <t>Specialty</t>
+  </si>
+  <si>
     <t>Low Range</t>
   </si>
   <si>
     <t>High Range</t>
   </si>
   <si>
-    <t>1c</t>
-  </si>
-  <si>
-    <t>2c</t>
-  </si>
-  <si>
-    <t>3c</t>
-  </si>
-  <si>
-    <t>4c</t>
-  </si>
-  <si>
-    <t>5c</t>
-  </si>
-  <si>
-    <t>6c</t>
-  </si>
-  <si>
-    <t>7c</t>
+    <t>pricing_1c</t>
+  </si>
+  <si>
+    <t>pricing_2c</t>
+  </si>
+  <si>
+    <t>pricing_3c</t>
+  </si>
+  <si>
+    <t>pricing_4c</t>
+  </si>
+  <si>
+    <t>pricing_5c</t>
+  </si>
+  <si>
+    <t>pricing_6c</t>
+  </si>
+  <si>
+    <t>pricing_7c</t>
   </si>
   <si>
     <t>range_low_1</t>
@@ -193,55 +203,40 @@
     <t>range_high</t>
   </si>
   <si>
-    <t>pricing_1c</t>
-  </si>
-  <si>
-    <t>pricing_2c</t>
-  </si>
-  <si>
-    <t>pricing_3c</t>
-  </si>
-  <si>
-    <t>pricing_4c</t>
-  </si>
-  <si>
-    <t>pricing_5c</t>
-  </si>
-  <si>
-    <t>pricing_6c</t>
-  </si>
-  <si>
-    <t>pricing_7c</t>
-  </si>
-  <si>
     <t>pricing_8c</t>
   </si>
   <si>
     <t>pricing_9c</t>
   </si>
   <si>
-    <t>4*4 Light</t>
-  </si>
-  <si>
-    <t>4*4 Dark</t>
-  </si>
-  <si>
-    <t>6*6 Light</t>
-  </si>
-  <si>
-    <t>6*6 Dark</t>
-  </si>
-  <si>
-    <t>10*10 Light</t>
-  </si>
-  <si>
-    <t>10*10 Dark</t>
-  </si>
-  <si>
-    <t>12*12 Light</t>
-  </si>
-  <si>
-    <t>12*12 Dark</t>
+    <t>Range Low</t>
+  </si>
+  <si>
+    <t>Range High</t>
+  </si>
+  <si>
+    <t>Light 4*4 </t>
+  </si>
+  <si>
+    <t>Dark 4*4 </t>
+  </si>
+  <si>
+    <t>Light 6*6 </t>
+  </si>
+  <si>
+    <t>Dark 6*6 </t>
+  </si>
+  <si>
+    <t> Light 10*10</t>
+  </si>
+  <si>
+    <t>Dark 10*10 </t>
+  </si>
+  <si>
+    <t>Light 12*12 </t>
+  </si>
+  <si>
+    <t>Dark 12*12 </t>
   </si>
   <si>
     <t>Percentage</t>
@@ -251,11 +246,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="1">
     <numFmt numFmtId="164" formatCode="GENERAL"/>
-    <numFmt numFmtId="165" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -283,6 +277,12 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -327,7 +327,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -336,8 +336,12 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -359,8 +363,8 @@
   </sheetPr>
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E10" activeCellId="0" sqref="E10"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B14" activeCellId="0" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -383,6 +387,32 @@
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5204081632653"/>
+  </cols>
+  <sheetData/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -397,8 +427,8 @@
   </sheetPr>
   <dimension ref="A1:R2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D15" activeCellId="0" sqref="D15"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="I1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="K11" activeCellId="0" sqref="K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -544,10 +574,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:R3"/>
+  <dimension ref="A1:R9"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E12" activeCellId="0" sqref="E12"/>
+      <selection pane="topLeft" activeCell="E21" activeCellId="0" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -602,13 +632,13 @@
       <c r="C2" s="0" t="n">
         <v>6</v>
       </c>
-      <c r="D2" s="2" t="b">
+      <c r="D2" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="E2" s="2" t="b">
+      <c r="E2" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="F2" s="2" t="b">
+      <c r="F2" s="2" t="n">
         <v>1</v>
       </c>
     </row>
@@ -623,13 +653,133 @@
         <v>7</v>
       </c>
       <c r="D3" s="2" t="n">
-        <v>2</v>
-      </c>
-      <c r="E3" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E3" s="2" t="n">
         <v>1</v>
       </c>
       <c r="F3" s="2" t="n">
-        <v>2</v>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="0" t="n">
+        <v>21</v>
+      </c>
+      <c r="C4" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="D4" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="E4" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F4" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="B5" s="0" t="n">
+        <v>22</v>
+      </c>
+      <c r="C5" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="D5" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F5" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="B6" s="0" t="n">
+        <v>23</v>
+      </c>
+      <c r="C6" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="D6" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="E6" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F6" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" s="0" t="n">
+        <v>24</v>
+      </c>
+      <c r="C7" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="D7" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E7" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F7" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="B8" s="0" t="n">
+        <v>25</v>
+      </c>
+      <c r="C8" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="D8" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E8" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F8" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" s="0" t="n">
+        <v>26</v>
+      </c>
+      <c r="C9" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="D9" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E9" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F9" s="0" t="n">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -648,23 +798,23 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:R3"/>
+  <dimension ref="A1:R11"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D17" activeCellId="0" sqref="D17"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.8112244897959"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.030612244898"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="10.4132653061225"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.89285714285714"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="9.43877551020408"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="10.4132653061225"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="7.77551020408163"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="7.21938775510204"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="7.77551020408163"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="12.5"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="10.8367346938776"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="11.530612244898"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="12.5"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="11.3928571428571"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="14.1632653061225"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="17.3622448979592"/>
     <col collapsed="false" hidden="false" max="11" min="10" style="0" width="11.5204081632653"/>
     <col collapsed="false" hidden="false" max="12" min="12" style="0" width="15.6938775510204"/>
     <col collapsed="false" hidden="false" max="13" min="13" style="0" width="21.5357142857143"/>
@@ -677,31 +827,31 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="R1" s="1"/>
     </row>
@@ -761,6 +911,238 @@
       </c>
       <c r="I3" s="0" t="n">
         <v>3.88</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="n">
+        <v>72</v>
+      </c>
+      <c r="B4" s="0" t="n">
+        <v>143</v>
+      </c>
+      <c r="C4" s="0" t="n">
+        <v>11.19</v>
+      </c>
+      <c r="D4" s="0" t="n">
+        <v>11.69</v>
+      </c>
+      <c r="E4" s="0" t="n">
+        <v>11.21</v>
+      </c>
+      <c r="F4" s="0" t="n">
+        <v>11.22</v>
+      </c>
+      <c r="G4" s="0" t="n">
+        <v>11.23</v>
+      </c>
+      <c r="H4" s="0" t="n">
+        <v>11.24</v>
+      </c>
+      <c r="I4" s="0" t="n">
+        <v>1.25</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="B5" s="0" t="n">
+        <v>215</v>
+      </c>
+      <c r="C5" s="0" t="n">
+        <v>11.19</v>
+      </c>
+      <c r="D5" s="0" t="n">
+        <v>11.2</v>
+      </c>
+      <c r="E5" s="0" t="n">
+        <v>10.11</v>
+      </c>
+      <c r="F5" s="0" t="n">
+        <v>10.12</v>
+      </c>
+      <c r="G5" s="0" t="n">
+        <v>11.13</v>
+      </c>
+      <c r="H5" s="0" t="n">
+        <v>10.14</v>
+      </c>
+      <c r="I5" s="0" t="n">
+        <v>10.15</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="n">
+        <v>216</v>
+      </c>
+      <c r="B6" s="0" t="n">
+        <v>287</v>
+      </c>
+      <c r="C6" s="0" t="n">
+        <v>10.8</v>
+      </c>
+      <c r="D6" s="0" t="n">
+        <v>10.1</v>
+      </c>
+      <c r="E6" s="0" t="n">
+        <v>10.21</v>
+      </c>
+      <c r="F6" s="0" t="n">
+        <v>10.22</v>
+      </c>
+      <c r="G6" s="0" t="n">
+        <v>10.23</v>
+      </c>
+      <c r="H6" s="0" t="n">
+        <v>10.24</v>
+      </c>
+      <c r="I6" s="0" t="n">
+        <v>10.25</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="n">
+        <v>288</v>
+      </c>
+      <c r="B7" s="0" t="n">
+        <v>431</v>
+      </c>
+      <c r="C7" s="0" t="n">
+        <v>10.66</v>
+      </c>
+      <c r="D7" s="0" t="n">
+        <v>10.2</v>
+      </c>
+      <c r="E7" s="0" t="n">
+        <v>10.68</v>
+      </c>
+      <c r="F7" s="0" t="n">
+        <v>10.69</v>
+      </c>
+      <c r="G7" s="0" t="n">
+        <v>10.7</v>
+      </c>
+      <c r="H7" s="0" t="n">
+        <v>10.71</v>
+      </c>
+      <c r="I7" s="0" t="n">
+        <v>10.72</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="n">
+        <v>432</v>
+      </c>
+      <c r="B8" s="0" t="n">
+        <v>575</v>
+      </c>
+      <c r="C8" s="0" t="n">
+        <v>10.65</v>
+      </c>
+      <c r="D8" s="0" t="n">
+        <v>10.67</v>
+      </c>
+      <c r="E8" s="0" t="n">
+        <v>11.2</v>
+      </c>
+      <c r="F8" s="0" t="n">
+        <v>11.3</v>
+      </c>
+      <c r="G8" s="0" t="n">
+        <v>11.4</v>
+      </c>
+      <c r="H8" s="0" t="n">
+        <v>11.5</v>
+      </c>
+      <c r="I8" s="0" t="n">
+        <v>11.6</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="n">
+        <v>576</v>
+      </c>
+      <c r="B9" s="0" t="n">
+        <v>863</v>
+      </c>
+      <c r="C9" s="0" t="n">
+        <v>10.44</v>
+      </c>
+      <c r="D9" s="0" t="n">
+        <v>11.1</v>
+      </c>
+      <c r="E9" s="0" t="n">
+        <v>11.13</v>
+      </c>
+      <c r="F9" s="0" t="n">
+        <v>11.14</v>
+      </c>
+      <c r="G9" s="0" t="n">
+        <v>11.15</v>
+      </c>
+      <c r="H9" s="0" t="n">
+        <v>11.16</v>
+      </c>
+      <c r="I9" s="0" t="n">
+        <v>11.17</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="n">
+        <v>864</v>
+      </c>
+      <c r="B10" s="0" t="n">
+        <v>1151</v>
+      </c>
+      <c r="C10" s="0" t="n">
+        <v>10.41</v>
+      </c>
+      <c r="D10" s="0" t="n">
+        <v>11.12</v>
+      </c>
+      <c r="E10" s="0" t="n">
+        <v>10.43</v>
+      </c>
+      <c r="F10" s="0" t="n">
+        <v>10.44</v>
+      </c>
+      <c r="G10" s="0" t="n">
+        <v>10.45</v>
+      </c>
+      <c r="H10" s="0" t="n">
+        <v>10.46</v>
+      </c>
+      <c r="I10" s="0" t="n">
+        <v>10.47</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="n">
+        <v>1152</v>
+      </c>
+      <c r="B11" s="0" t="n">
+        <v>2999</v>
+      </c>
+      <c r="C11" s="0" t="n">
+        <v>10.31</v>
+      </c>
+      <c r="D11" s="0" t="n">
+        <v>10.42</v>
+      </c>
+      <c r="E11" s="0" t="n">
+        <v>10.33</v>
+      </c>
+      <c r="F11" s="0" t="n">
+        <v>1034</v>
+      </c>
+      <c r="G11" s="0" t="n">
+        <v>10.35</v>
+      </c>
+      <c r="H11" s="0" t="n">
+        <v>10.36</v>
+      </c>
+      <c r="I11" s="0" t="n">
+        <v>10.37</v>
       </c>
     </row>
   </sheetData>
@@ -779,23 +1161,23 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:R3"/>
+  <dimension ref="A1:R11"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D17" activeCellId="0" sqref="D17"/>
+      <selection pane="topLeft" activeCell="F20" activeCellId="0" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.8112244897959"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.030612244898"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="10.4132653061225"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.89285714285714"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="9.43877551020408"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="10.4132653061225"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="7.77551020408163"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="7.21938775510204"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="7.77551020408163"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="12.6377551020408"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="11.8061224489796"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="12.3673469387755"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="12.5"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="12.780612244898"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="11.8061224489796"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="14.030612244898"/>
     <col collapsed="false" hidden="false" max="11" min="10" style="0" width="11.5204081632653"/>
     <col collapsed="false" hidden="false" max="12" min="12" style="0" width="15.6938775510204"/>
     <col collapsed="false" hidden="false" max="13" min="13" style="0" width="21.5357142857143"/>
@@ -808,31 +1190,31 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="R1" s="1"/>
     </row>
@@ -892,6 +1274,238 @@
       </c>
       <c r="I3" s="0" t="n">
         <v>3.88</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="n">
+        <v>72</v>
+      </c>
+      <c r="B4" s="0" t="n">
+        <v>143</v>
+      </c>
+      <c r="C4" s="0" t="n">
+        <v>11.19</v>
+      </c>
+      <c r="D4" s="0" t="n">
+        <v>11.69</v>
+      </c>
+      <c r="E4" s="0" t="n">
+        <v>11.21</v>
+      </c>
+      <c r="F4" s="0" t="n">
+        <v>11.22</v>
+      </c>
+      <c r="G4" s="0" t="n">
+        <v>11.23</v>
+      </c>
+      <c r="H4" s="0" t="n">
+        <v>11.24</v>
+      </c>
+      <c r="I4" s="0" t="n">
+        <v>1.25</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="B5" s="0" t="n">
+        <v>215</v>
+      </c>
+      <c r="C5" s="0" t="n">
+        <v>11.19</v>
+      </c>
+      <c r="D5" s="0" t="n">
+        <v>11.2</v>
+      </c>
+      <c r="E5" s="0" t="n">
+        <v>10.11</v>
+      </c>
+      <c r="F5" s="0" t="n">
+        <v>10.12</v>
+      </c>
+      <c r="G5" s="0" t="n">
+        <v>11.13</v>
+      </c>
+      <c r="H5" s="0" t="n">
+        <v>10.14</v>
+      </c>
+      <c r="I5" s="0" t="n">
+        <v>10.15</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="n">
+        <v>216</v>
+      </c>
+      <c r="B6" s="0" t="n">
+        <v>287</v>
+      </c>
+      <c r="C6" s="0" t="n">
+        <v>10.8</v>
+      </c>
+      <c r="D6" s="0" t="n">
+        <v>10.1</v>
+      </c>
+      <c r="E6" s="0" t="n">
+        <v>10.21</v>
+      </c>
+      <c r="F6" s="0" t="n">
+        <v>10.22</v>
+      </c>
+      <c r="G6" s="0" t="n">
+        <v>10.23</v>
+      </c>
+      <c r="H6" s="0" t="n">
+        <v>10.24</v>
+      </c>
+      <c r="I6" s="0" t="n">
+        <v>10.25</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="n">
+        <v>288</v>
+      </c>
+      <c r="B7" s="0" t="n">
+        <v>431</v>
+      </c>
+      <c r="C7" s="0" t="n">
+        <v>10.66</v>
+      </c>
+      <c r="D7" s="0" t="n">
+        <v>10.2</v>
+      </c>
+      <c r="E7" s="0" t="n">
+        <v>10.68</v>
+      </c>
+      <c r="F7" s="0" t="n">
+        <v>10.69</v>
+      </c>
+      <c r="G7" s="0" t="n">
+        <v>10.7</v>
+      </c>
+      <c r="H7" s="0" t="n">
+        <v>10.71</v>
+      </c>
+      <c r="I7" s="0" t="n">
+        <v>10.72</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="n">
+        <v>432</v>
+      </c>
+      <c r="B8" s="0" t="n">
+        <v>575</v>
+      </c>
+      <c r="C8" s="0" t="n">
+        <v>10.65</v>
+      </c>
+      <c r="D8" s="0" t="n">
+        <v>10.67</v>
+      </c>
+      <c r="E8" s="0" t="n">
+        <v>11.2</v>
+      </c>
+      <c r="F8" s="0" t="n">
+        <v>11.3</v>
+      </c>
+      <c r="G8" s="0" t="n">
+        <v>11.4</v>
+      </c>
+      <c r="H8" s="0" t="n">
+        <v>11.5</v>
+      </c>
+      <c r="I8" s="0" t="n">
+        <v>11.6</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="n">
+        <v>576</v>
+      </c>
+      <c r="B9" s="0" t="n">
+        <v>863</v>
+      </c>
+      <c r="C9" s="0" t="n">
+        <v>10.44</v>
+      </c>
+      <c r="D9" s="0" t="n">
+        <v>11.1</v>
+      </c>
+      <c r="E9" s="0" t="n">
+        <v>11.13</v>
+      </c>
+      <c r="F9" s="0" t="n">
+        <v>11.14</v>
+      </c>
+      <c r="G9" s="0" t="n">
+        <v>11.15</v>
+      </c>
+      <c r="H9" s="0" t="n">
+        <v>11.16</v>
+      </c>
+      <c r="I9" s="0" t="n">
+        <v>11.17</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="n">
+        <v>864</v>
+      </c>
+      <c r="B10" s="0" t="n">
+        <v>1151</v>
+      </c>
+      <c r="C10" s="0" t="n">
+        <v>10.41</v>
+      </c>
+      <c r="D10" s="0" t="n">
+        <v>11.12</v>
+      </c>
+      <c r="E10" s="0" t="n">
+        <v>10.43</v>
+      </c>
+      <c r="F10" s="0" t="n">
+        <v>10.44</v>
+      </c>
+      <c r="G10" s="0" t="n">
+        <v>10.45</v>
+      </c>
+      <c r="H10" s="0" t="n">
+        <v>10.46</v>
+      </c>
+      <c r="I10" s="0" t="n">
+        <v>10.47</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="n">
+        <v>1152</v>
+      </c>
+      <c r="B11" s="0" t="n">
+        <v>2999</v>
+      </c>
+      <c r="C11" s="0" t="n">
+        <v>10.31</v>
+      </c>
+      <c r="D11" s="0" t="n">
+        <v>10.42</v>
+      </c>
+      <c r="E11" s="0" t="n">
+        <v>10.33</v>
+      </c>
+      <c r="F11" s="0" t="n">
+        <v>1034</v>
+      </c>
+      <c r="G11" s="0" t="n">
+        <v>10.35</v>
+      </c>
+      <c r="H11" s="0" t="n">
+        <v>10.36</v>
+      </c>
+      <c r="I11" s="0" t="n">
+        <v>10.37</v>
       </c>
     </row>
   </sheetData>
@@ -913,7 +1527,7 @@
   <dimension ref="A1:R2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D17" activeCellId="0" sqref="D17"/>
+      <selection pane="topLeft" activeCell="B32" activeCellId="0" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -932,58 +1546,58 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1058,10 +1672,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:K3"/>
+  <dimension ref="A1:K4"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E19" activeCellId="0" sqref="E19"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B10" activeCellId="0" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -1082,37 +1696,37 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>56</v>
+        <v>32</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>57</v>
+        <v>33</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>58</v>
+        <v>34</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>60</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1183,6 +1797,41 @@
       </c>
       <c r="K3" s="0" t="n">
         <v>9.5</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="n">
+        <v>24</v>
+      </c>
+      <c r="B4" s="0" t="n">
+        <v>71</v>
+      </c>
+      <c r="C4" s="0" t="n">
+        <v>12.48</v>
+      </c>
+      <c r="D4" s="0" t="n">
+        <v>12.85</v>
+      </c>
+      <c r="E4" s="0" t="n">
+        <v>13.23</v>
+      </c>
+      <c r="F4" s="0" t="n">
+        <v>13.6</v>
+      </c>
+      <c r="G4" s="0" t="n">
+        <v>13.98</v>
+      </c>
+      <c r="H4" s="0" t="n">
+        <v>14.35</v>
+      </c>
+      <c r="I4" s="0" t="n">
+        <v>14.73</v>
+      </c>
+      <c r="J4" s="0" t="n">
+        <v>15.1</v>
+      </c>
+      <c r="K4" s="0" t="n">
+        <v>16.1</v>
       </c>
     </row>
   </sheetData>
@@ -1201,10 +1850,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:R3"/>
+  <dimension ref="A1:R6"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B11" activeCellId="0" sqref="B11"/>
+      <selection pane="topLeft" activeCell="H17" activeCellId="0" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -1230,35 +1879,35 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>28</v>
+      <c r="A1" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>62</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>70</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>72</v>
       </c>
       <c r="R1" s="1"/>
     </row>
@@ -1320,10 +1969,106 @@
         <v>22</v>
       </c>
       <c r="I3" s="0" t="n">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="J3" s="0" t="n">
         <v>24</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="C4" s="0" t="n">
+        <v>21</v>
+      </c>
+      <c r="D4" s="0" t="n">
+        <v>27</v>
+      </c>
+      <c r="E4" s="0" t="n">
+        <v>25</v>
+      </c>
+      <c r="F4" s="0" t="n">
+        <v>28</v>
+      </c>
+      <c r="G4" s="0" t="n">
+        <v>27</v>
+      </c>
+      <c r="H4" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="I4" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="J4" s="0" t="n">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="B5" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="C5" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="D5" s="0" t="n">
+        <v>25</v>
+      </c>
+      <c r="E5" s="0" t="n">
+        <v>26</v>
+      </c>
+      <c r="F5" s="0" t="n">
+        <v>24</v>
+      </c>
+      <c r="G5" s="0" t="n">
+        <v>27</v>
+      </c>
+      <c r="H5" s="0" t="n">
+        <v>26</v>
+      </c>
+      <c r="I5" s="0" t="n">
+        <v>29</v>
+      </c>
+      <c r="J5" s="0" t="n">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="B6" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="C6" s="0" t="n">
+        <v>19</v>
+      </c>
+      <c r="D6" s="0" t="n">
+        <v>25</v>
+      </c>
+      <c r="E6" s="0" t="n">
+        <v>23</v>
+      </c>
+      <c r="F6" s="0" t="n">
+        <v>26</v>
+      </c>
+      <c r="G6" s="0" t="n">
+        <v>25</v>
+      </c>
+      <c r="H6" s="0" t="n">
+        <v>26</v>
+      </c>
+      <c r="I6" s="0" t="n">
+        <v>28</v>
+      </c>
+      <c r="J6" s="0" t="n">
+        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -1342,10 +2087,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:R3"/>
+  <dimension ref="A1:R5"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D20" activeCellId="0" sqref="D20"/>
+      <selection pane="topLeft" activeCell="D16" activeCellId="0" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -1371,14 +2116,14 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>28</v>
+      <c r="A1" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>62</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="R1" s="1"/>
     </row>
@@ -1402,6 +2147,28 @@
       </c>
       <c r="C3" s="0" t="n">
         <v>80</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="n">
+        <v>201</v>
+      </c>
+      <c r="B4" s="0" t="n">
+        <v>300</v>
+      </c>
+      <c r="C4" s="0" t="n">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="n">
+        <v>301</v>
+      </c>
+      <c r="B5" s="0" t="n">
+        <v>400</v>
+      </c>
+      <c r="C5" s="0" t="n">
+        <v>100</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
STO-316 #comment Add till 16c in 'Screen Print Primary' and 'Screen Print Secondary' in price grid #time 6h Add till 16c in 'Screen Print Primary' and 'Screen Print Secondary' in price grid
</commit_message>
<xml_diff>
--- a/api/addpricegrid.xlsx
+++ b/api/addpricegrid.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="208" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="208" firstSheet="0" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="PriceGrid" sheetId="1" state="visible" r:id="rId2"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="79">
   <si>
     <t>Name</t>
   </si>
@@ -143,6 +143,33 @@
     <t>pricing_7c</t>
   </si>
   <si>
+    <t>pricing_8c</t>
+  </si>
+  <si>
+    <t>pricing_9c</t>
+  </si>
+  <si>
+    <t>pricing_10c</t>
+  </si>
+  <si>
+    <t>pricing_11c</t>
+  </si>
+  <si>
+    <t>pricing_12c</t>
+  </si>
+  <si>
+    <t>pricing_13c</t>
+  </si>
+  <si>
+    <t>pricing_14c</t>
+  </si>
+  <si>
+    <t>pricing_15c</t>
+  </si>
+  <si>
+    <t>pricing_16c</t>
+  </si>
+  <si>
     <t>range_low_1</t>
   </si>
   <si>
@@ -203,40 +230,34 @@
     <t>range_high</t>
   </si>
   <si>
-    <t>pricing_8c</t>
-  </si>
-  <si>
-    <t>pricing_9c</t>
-  </si>
-  <si>
     <t>Range Low</t>
   </si>
   <si>
     <t>Range High</t>
   </si>
   <si>
-    <t>Light 4*4 </t>
-  </si>
-  <si>
-    <t>Dark 4*4 </t>
-  </si>
-  <si>
-    <t>Light 6*6 </t>
-  </si>
-  <si>
-    <t>Dark 6*6 </t>
-  </si>
-  <si>
-    <t> Light 10*10</t>
-  </si>
-  <si>
-    <t>Dark 10*10 </t>
-  </si>
-  <si>
-    <t>Light 12*12 </t>
-  </si>
-  <si>
-    <t>Dark 12*12 </t>
+    <t>Light 4*4</t>
+  </si>
+  <si>
+    <t>Dark 4*4</t>
+  </si>
+  <si>
+    <t>Light 6*6</t>
+  </si>
+  <si>
+    <t>Dark 6*6</t>
+  </si>
+  <si>
+    <t>Light 10*10</t>
+  </si>
+  <si>
+    <t>Dark 10*10</t>
+  </si>
+  <si>
+    <t>Light 12*12</t>
+  </si>
+  <si>
+    <t>Dark 12*12</t>
   </si>
   <si>
     <t>Percentage</t>
@@ -249,7 +270,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="GENERAL"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -277,12 +298,6 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -327,20 +342,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="2">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -363,7 +370,7 @@
   </sheetPr>
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B14" activeCellId="0" sqref="B14"/>
     </sheetView>
   </sheetViews>
@@ -632,13 +639,13 @@
       <c r="C2" s="0" t="n">
         <v>6</v>
       </c>
-      <c r="D2" s="2" t="n">
+      <c r="D2" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="E2" s="2" t="n">
+      <c r="E2" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="F2" s="2" t="n">
+      <c r="F2" s="0" t="n">
         <v>1</v>
       </c>
     </row>
@@ -652,13 +659,13 @@
       <c r="C3" s="0" t="n">
         <v>7</v>
       </c>
-      <c r="D3" s="2" t="n">
+      <c r="D3" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="E3" s="2" t="n">
+      <c r="E3" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="F3" s="2" t="n">
+      <c r="F3" s="0" t="n">
         <v>0</v>
       </c>
     </row>
@@ -672,7 +679,7 @@
       <c r="C4" s="0" t="n">
         <v>8</v>
       </c>
-      <c r="D4" s="2" t="n">
+      <c r="D4" s="0" t="n">
         <v>1</v>
       </c>
       <c r="E4" s="0" t="n">
@@ -692,7 +699,7 @@
       <c r="C5" s="0" t="n">
         <v>9</v>
       </c>
-      <c r="D5" s="2" t="n">
+      <c r="D5" s="0" t="n">
         <v>0</v>
       </c>
       <c r="E5" s="0" t="n">
@@ -712,7 +719,7 @@
       <c r="C6" s="0" t="n">
         <v>10</v>
       </c>
-      <c r="D6" s="2" t="n">
+      <c r="D6" s="0" t="n">
         <v>1</v>
       </c>
       <c r="E6" s="0" t="n">
@@ -732,7 +739,7 @@
       <c r="C7" s="0" t="n">
         <v>11</v>
       </c>
-      <c r="D7" s="2" t="n">
+      <c r="D7" s="0" t="n">
         <v>0</v>
       </c>
       <c r="E7" s="0" t="n">
@@ -752,7 +759,7 @@
       <c r="C8" s="0" t="n">
         <v>12</v>
       </c>
-      <c r="D8" s="2" t="n">
+      <c r="D8" s="0" t="n">
         <v>0</v>
       </c>
       <c r="E8" s="0" t="n">
@@ -772,7 +779,7 @@
       <c r="C9" s="0" t="n">
         <v>13</v>
       </c>
-      <c r="D9" s="2" t="n">
+      <c r="D9" s="0" t="n">
         <v>0</v>
       </c>
       <c r="E9" s="0" t="n">
@@ -800,8 +807,8 @@
   </sheetPr>
   <dimension ref="A1:R11"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="H1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J1" activeCellId="0" sqref="J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -853,7 +860,33 @@
       <c r="I1" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="R1" s="1"/>
+      <c r="J1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="n">
@@ -1163,8 +1196,8 @@
   </sheetPr>
   <dimension ref="A1:R11"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F20" activeCellId="0" sqref="F20"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="O12" activeCellId="0" sqref="O12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -1216,7 +1249,33 @@
       <c r="I1" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="R1" s="1"/>
+      <c r="J1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="n">
@@ -1546,58 +1605,58 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>40</v>
+        <v>49</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>42</v>
+        <v>51</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>43</v>
+        <v>52</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>45</v>
+        <v>54</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>46</v>
+        <v>55</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>47</v>
+        <v>56</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>48</v>
+        <v>57</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>49</v>
+        <v>58</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>50</v>
+        <v>59</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>51</v>
+        <v>60</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>52</v>
+        <v>61</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>53</v>
+        <v>62</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>54</v>
+        <v>63</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>55</v>
+        <v>64</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>56</v>
+        <v>65</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1696,10 +1755,10 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>57</v>
+        <v>66</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>58</v>
+        <v>67</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>32</v>
@@ -1723,10 +1782,10 @@
         <v>38</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>59</v>
+        <v>39</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>60</v>
+        <v>40</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1879,35 +1938,35 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>62</v>
+      <c r="A1" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>69</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>63</v>
+        <v>70</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>64</v>
+        <v>71</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>65</v>
+        <v>72</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>66</v>
+        <v>73</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>67</v>
+        <v>74</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>68</v>
+        <v>75</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>69</v>
+        <v>76</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>70</v>
+        <v>77</v>
       </c>
       <c r="R1" s="1"/>
     </row>
@@ -2116,14 +2175,14 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>62</v>
+      <c r="A1" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>69</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>71</v>
+        <v>78</v>
       </c>
       <c r="R1" s="1"/>
     </row>

</xml_diff>